<commit_message>
show the current working foler
It is used to deploy and run this un-attend job in Orchestrator
</commit_message>
<xml_diff>
--- a/UIAutomation/Transaction.xlsx
+++ b/UIAutomation/Transaction.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hongphucvi\Documents\GitHub\RPA\UIAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7DF399F-C639-438A-8683-56CB417DF580}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E5CE837-CC94-4AB1-A50C-5C6DD3156C68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="1080" windowWidth="13680" windowHeight="7245" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="13680" windowHeight="7245" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -358,7 +358,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -394,9 +394,6 @@
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>640808</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>